<commit_message>
wip: improved users seeds
</commit_message>
<xml_diff>
--- a/graphql/db/users.xlsx
+++ b/graphql/db/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B054513-0479-624F-86CD-839852260BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7957C536-0590-6B45-B6B5-55C8B6638937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9680" yWindow="4480" windowWidth="26840" windowHeight="15940" xr2:uid="{BD1E2374-5E66-0C45-A2D1-38630B7737D9}"/>
   </bookViews>
@@ -53,18 +53,12 @@
     <t>admin@wildwheeladventures.cz</t>
   </si>
   <si>
-    <t>+420 123 456 789</t>
-  </si>
-  <si>
     <t>wild-whieel</t>
   </si>
   <si>
     <t>admin@glidequesttours.cz</t>
   </si>
   <si>
-    <t>+420 987 654 321</t>
-  </si>
-  <si>
     <t>glide-quest</t>
   </si>
   <si>
@@ -87,13 +81,19 @@
   </si>
   <si>
     <t>mikhail@dorokhovich.ru</t>
+  </si>
+  <si>
+    <t>+420296182740</t>
+  </si>
+  <si>
+    <t>+420255708904</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,9 +111,12 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF374151"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,11 +140,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -460,121 +464,122 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>